<commit_message>
chore: finalize phase2.1 verification pack, glossary sync, and docs/notion links
</commit_message>
<xml_diff>
--- a/07_MVP_GLOSSARY_CEO_KR.xlsx
+++ b/07_MVP_GLOSSARY_CEO_KR.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="흐름설명" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="에러코드해설" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10분점검표" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="경영진1페이지요약" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'용어사전'!$A$4:$J$24</definedName>
@@ -22,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,8 +65,34 @@
       <color rgb="0034495E"/>
       <sz val="12"/>
     </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <color rgb="001F2937"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <b val="1"/>
+      <color rgb="001F365C"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <b val="1"/>
+      <color rgb="001E4D2B"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="18">
     <fill>
       <patternFill/>
     </fill>
@@ -127,8 +154,33 @@
         <fgColor rgb="005E548E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EAF2FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EEF6EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8F9FC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF4E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -150,11 +202,69 @@
         <color rgb="00D8E1EB"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00D9DCE3"/>
+      </left>
+      <right style="thin">
+        <color rgb="00D9DCE3"/>
+      </right>
+      <top style="thin">
+        <color rgb="00D9DCE3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00D9DCE3"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00D9DCE3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00D9DCE3"/>
+      </right>
+      <top style="thin">
+        <color rgb="00D9DCE3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00D9DCE3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00D9DCE3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00D9DCE3"/>
+      </right>
+      <top style="thin">
+        <color rgb="00D9DCE3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00D9DCE3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -204,6 +314,31 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,7 +738,7 @@
     <row r="2" ht="42" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>목적: 기술 용어를 쉬운 한국어로 이해하고, 경영진이 리스크/통제 포인트를 즉시 판단하도록 지원 (생성 시각: 2026-02-18 14:48)</t>
+          <t>목적: 기술 용어를 쉬운 한국어로 이해하고, 경영진이 리스크/통제 포인트를 즉시 판단하도록 지원 (생성 시각: 2026-02-18 20:03)</t>
         </is>
       </c>
       <c r="K2" s="2" t="n"/>
@@ -1758,126 +1893,438 @@
       <c r="L24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n"/>
-      <c r="B25" s="2" t="n"/>
-      <c r="C25" s="2" t="n"/>
-      <c r="D25" s="2" t="n"/>
-      <c r="E25" s="2" t="n"/>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="2" t="n"/>
-      <c r="H25" s="2" t="n"/>
-      <c r="I25" s="2" t="n"/>
-      <c r="J25" s="2" t="n"/>
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>운영</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>Mock LLM(데모 프로파일)</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>데모 재현성을 위해 동일한 계약 JSON을 안정적으로 반환하는 모의 모델</t>
+        </is>
+      </c>
+      <c r="D25" s="7" t="inlineStr">
+        <is>
+          <t>데모/검증 프로파일(APP_LLM_PROVIDER=mock)</t>
+        </is>
+      </c>
+      <c r="E25" s="7" t="inlineStr">
+        <is>
+          <t>데모 변동성을 줄여 증빙 재현성을 높임</t>
+        </is>
+      </c>
+      <c r="F25" s="7" t="inlineStr">
+        <is>
+          <t>같은 질문에서 동일한 citation 흐름 재현</t>
+        </is>
+      </c>
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>운영 경로는 승인된 실제 Provider만 사용</t>
+        </is>
+      </c>
+      <c r="H25" s="7" t="inlineStr">
+        <is>
+          <t>AI-009-422-SCHEMA, AI-009-409-CITATION</t>
+        </is>
+      </c>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>Verify demo profile and production profile are separated</t>
+        </is>
+      </c>
+      <c r="J25" s="8" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
       <c r="K25" s="2" t="n"/>
       <c r="L25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n"/>
-      <c r="B26" s="2" t="n"/>
-      <c r="C26" s="2" t="n"/>
-      <c r="D26" s="2" t="n"/>
-      <c r="E26" s="2" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="2" t="n"/>
-      <c r="H26" s="2" t="n"/>
-      <c r="I26" s="2" t="n"/>
-      <c r="J26" s="2" t="n"/>
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>품질게이트</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="inlineStr">
+        <is>
+          <t>Citation 무결성 검사</t>
+        </is>
+      </c>
+      <c r="C26" s="7" t="inlineStr">
+        <is>
+          <t>모델이 제시한 citation chunk_id가 실제 검색 결과에 존재하는지 서버가 최종 검증</t>
+        </is>
+      </c>
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>MessageGenerationService 최종 검증 게이트</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>허위 출처 노출을 차단해 신뢰도 유지</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>미조회 chunk_id가 나오면 safe_response로 전환</t>
+        </is>
+      </c>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>모델 출력을 그대로 신뢰하면 안 됨</t>
+        </is>
+      </c>
+      <c r="H26" s="7" t="inlineStr">
+        <is>
+          <t>AI-009-409-CITATION</t>
+        </is>
+      </c>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>Compare retrieval chunk set vs citation chunk_id list</t>
+        </is>
+      </c>
+      <c r="J26" s="8" t="inlineStr">
+        <is>
+          <t>Highest</t>
+        </is>
+      </c>
       <c r="K26" s="2" t="n"/>
       <c r="L26" s="2" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n"/>
-      <c r="B27" s="2" t="n"/>
-      <c r="C27" s="2" t="n"/>
-      <c r="D27" s="2" t="n"/>
-      <c r="E27" s="2" t="n"/>
-      <c r="F27" s="2" t="n"/>
-      <c r="G27" s="2" t="n"/>
-      <c r="H27" s="2" t="n"/>
-      <c r="I27" s="2" t="n"/>
-      <c r="J27" s="2" t="n"/>
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>관측</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>UUID Trace 정책</t>
+        </is>
+      </c>
+      <c r="C27" s="7" t="inlineStr">
+        <is>
+          <t>X-Trace-Id를 UUID 형식으로만 허용하고, 위반 시 요청 거부</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>TraceIdFilter + 표준 오류 응답</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>HTTP/SSE/DB를 동일 추적키로 묶어 장애 분석 정확도 확보</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>비정상 trace_id는 409로 즉시 차단</t>
+        </is>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>중간 계층 정규화 불일치로 추적이 끊기지 않게 방지</t>
+        </is>
+      </c>
+      <c r="H27" s="7" t="inlineStr">
+        <is>
+          <t>SYS-004-409-TRACE</t>
+        </is>
+      </c>
+      <c r="I27" s="7" t="inlineStr">
+        <is>
+          <t>Send non-UUID header and confirm policy rejection</t>
+        </is>
+      </c>
+      <c r="J27" s="8" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
       <c r="K27" s="2" t="n"/>
       <c r="L27" s="2" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n"/>
-      <c r="B28" s="2" t="n"/>
-      <c r="C28" s="2" t="n"/>
-      <c r="D28" s="2" t="n"/>
-      <c r="E28" s="2" t="n"/>
-      <c r="F28" s="2" t="n"/>
-      <c r="G28" s="2" t="n"/>
-      <c r="H28" s="2" t="n"/>
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>거버넌스</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>SSOT(단일 진실원천)</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
+          <t>PASS/FAIL 판정을 한 문서(04_TEST_RESULTS.md) 기준으로만 관리하는 원칙</t>
+        </is>
+      </c>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>검증팩 문서 00/03/04/06/PHASE2</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>문서 간 판정 충돌로 인한 의사결정 오류 방지</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>요약 문서는 04를 그대로 요약만 수행</t>
+        </is>
+      </c>
+      <c r="G28" s="7" t="inlineStr">
+        <is>
+          <t>요약 문서가 04와 다르면 즉시 실패 처리</t>
+        </is>
+      </c>
+      <c r="H28" s="7" t="inlineStr">
+        <is>
+          <t>VER-CONSIST-001</t>
+        </is>
+      </c>
       <c r="I28" s="2" t="n"/>
       <c r="J28" s="2" t="n"/>
       <c r="K28" s="2" t="n"/>
       <c r="L28" s="2" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n"/>
-      <c r="B29" s="2" t="n"/>
-      <c r="C29" s="2" t="n"/>
-      <c r="D29" s="2" t="n"/>
-      <c r="E29" s="2" t="n"/>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="2" t="n"/>
-      <c r="H29" s="2" t="n"/>
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>운영통제</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>Branch Protection</t>
+        </is>
+      </c>
+      <c r="C29" s="7" t="inlineStr">
+        <is>
+          <t>필수 CI 체크가 통과되지 않으면 main 병합을 막는 저장소 보호 규칙</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>GitHub Branch Rule + Required check</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>사람 실수로 미검증 코드가 배포되는 리스크 차단</t>
+        </is>
+      </c>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>mvp-demo-verify 실패 시 Merge 버튼 비활성화</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>설정 누락 시 정책이 있어도 강제력 없음</t>
+        </is>
+      </c>
+      <c r="H29" s="7" t="inlineStr">
+        <is>
+          <t>mvp-demo-verify / verify</t>
+        </is>
+      </c>
       <c r="I29" s="2" t="n"/>
       <c r="J29" s="2" t="n"/>
       <c r="K29" s="2" t="n"/>
       <c r="L29" s="2" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n"/>
-      <c r="B30" s="2" t="n"/>
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="2" t="n"/>
-      <c r="E30" s="2" t="n"/>
-      <c r="F30" s="2" t="n"/>
-      <c r="G30" s="2" t="n"/>
-      <c r="H30" s="2" t="n"/>
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>검증자동화</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>Verification Pack Consistency Gate</t>
+        </is>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>문서 상태표와 증빙 파일 존재를 자동 대조해 모순을 차단하는 스크립트</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>scripts/assert_verification_pack_consistency.ps1</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>증빙 없는 PASS를 구조적으로 방지</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>PASS인데 artifact 파일이 없으면 즉시 실패</t>
+        </is>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>node_modules 같은 외부 파일은 중복 검사에서 제외 필요</t>
+        </is>
+      </c>
+      <c r="H30" s="7" t="inlineStr">
+        <is>
+          <t>VER-CONSIST-001</t>
+        </is>
+      </c>
       <c r="I30" s="2" t="n"/>
       <c r="J30" s="2" t="n"/>
       <c r="K30" s="2" t="n"/>
       <c r="L30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n"/>
-      <c r="B31" s="2" t="n"/>
-      <c r="C31" s="2" t="n"/>
-      <c r="D31" s="2" t="n"/>
-      <c r="E31" s="2" t="n"/>
-      <c r="F31" s="2" t="n"/>
-      <c r="G31" s="2" t="n"/>
-      <c r="H31" s="2" t="n"/>
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>보안</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <t>Artifact Sanitization Scan</t>
+        </is>
+      </c>
+      <c r="C31" s="7" t="inlineStr">
+        <is>
+          <t>아티팩트 내 토큰/이메일/전화번호 등 민감정보 패턴을 사전 탐지하는 스캔</t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>scripts/scan_artifacts_for_secrets_and_pii.ps1</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>보고/공유 단계에서 2차 유출을 예방</t>
+        </is>
+      </c>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>Bearer/JWT/이메일 패턴 검출 시 게이트 실패</t>
+        </is>
+      </c>
+      <c r="G31" s="7" t="inlineStr">
+        <is>
+          <t>과도한 오탐은 allowlist로 통제</t>
+        </is>
+      </c>
+      <c r="H31" s="7" t="inlineStr">
+        <is>
+          <t>SEC-ARTIFACT-SCAN-001</t>
+        </is>
+      </c>
       <c r="I31" s="2" t="n"/>
       <c r="J31" s="2" t="n"/>
       <c r="K31" s="2" t="n"/>
       <c r="L31" s="2" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n"/>
-      <c r="B32" s="2" t="n"/>
-      <c r="C32" s="2" t="n"/>
-      <c r="D32" s="2" t="n"/>
-      <c r="E32" s="2" t="n"/>
-      <c r="F32" s="2" t="n"/>
-      <c r="G32" s="2" t="n"/>
-      <c r="H32" s="2" t="n"/>
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>성능/동시성</t>
+        </is>
+      </c>
+      <c r="B32" s="7" t="inlineStr">
+        <is>
+          <t>SSE 실한도 검증</t>
+        </is>
+      </c>
+      <c r="C32" s="7" t="inlineStr">
+        <is>
+          <t>강제 limit=0 테스트 외에 운영 한도(limit=2)에서도 3번째 연결이 429인지 검증</t>
+        </is>
+      </c>
+      <c r="D32" s="7" t="inlineStr">
+        <is>
+          <t>run_sse_concurrency_real_limit_test.ps1</t>
+        </is>
+      </c>
+      <c r="E32" s="7" t="inlineStr">
+        <is>
+          <t>현실적인 부하 조건에서 보호장치 유효성 확인</t>
+        </is>
+      </c>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t>동시 3연결 시 3번째가 API-008-429-SSE</t>
+        </is>
+      </c>
+      <c r="G32" s="7" t="inlineStr">
+        <is>
+          <t>테스트를 위해 스트림 유지시간(APP_BUDGET_SSE_HOLD_MS) 설정 필요</t>
+        </is>
+      </c>
+      <c r="H32" s="7" t="inlineStr">
+        <is>
+          <t>SSE-CONC-REAL-001</t>
+        </is>
+      </c>
       <c r="I32" s="2" t="n"/>
       <c r="J32" s="2" t="n"/>
       <c r="K32" s="2" t="n"/>
       <c r="L32" s="2" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n"/>
-      <c r="B33" s="2" t="n"/>
-      <c r="C33" s="2" t="n"/>
-      <c r="D33" s="2" t="n"/>
-      <c r="E33" s="2" t="n"/>
-      <c r="F33" s="2" t="n"/>
-      <c r="G33" s="2" t="n"/>
-      <c r="H33" s="2" t="n"/>
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>런타임 표준</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>Node 22.12.0 고정</t>
+        </is>
+      </c>
+      <c r="C33" s="7" t="inlineStr">
+        <is>
+          <t>프론트 빌드/CI 재현성을 위해 Node 버전을 22.12.0으로 고정</t>
+        </is>
+      </c>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>.nvmrc, CI setup-node, verify_all</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>개발자 환경 차이로 인한 빌드 불일치 감소</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>CI는 22가 아니면 실패</t>
+        </is>
+      </c>
+      <c r="G33" s="7" t="inlineStr">
+        <is>
+          <t>로컬 오버라이드는 임시 진단 목적에만 사용</t>
+        </is>
+      </c>
+      <c r="H33" s="7" t="inlineStr">
+        <is>
+          <t>node_version_check.txt</t>
+        </is>
+      </c>
       <c r="I33" s="2" t="n"/>
       <c r="J33" s="2" t="n"/>
       <c r="K33" s="2" t="n"/>
@@ -8740,33 +9187,117 @@
       <c r="H9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" s="2" t="n"/>
-      <c r="G10" s="2" t="n"/>
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>7. 문서 정합성 게이트</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>검증 결과 대시보드 확인</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>04 결과표와 요약문서 상태표를 자동 대조</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>게이트 실패 시 릴리즈 보류</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>SSOT Consistency</t>
+        </is>
+      </c>
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>PASS인데 증빙 파일이 실제 존재하는가?</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/e2e_runner_stdout.txt</t>
+        </is>
+      </c>
       <c r="H10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
-      <c r="F11" s="2" t="n"/>
-      <c r="G11" s="2" t="n"/>
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>8. 아티팩트 보안 스캔</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>증빙 공유 전 최종 점검</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>토큰/PII 패턴 스캔 후 공유 가능 여부 판단</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>검출 시 공유 중단/마스킹 재작업</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>Artifact Sanitization</t>
+        </is>
+      </c>
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>공유 파일에 원문 이메일·토큰이 없는가?</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/artifact_sanitization_scan.txt</t>
+        </is>
+      </c>
       <c r="H11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="n"/>
-      <c r="F12" s="2" t="n"/>
-      <c r="G12" s="2" t="n"/>
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>9. 브랜치 보호 확인</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>배포 전 머지 정책 확인</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>필수 체크(required check) 등록 상태 점검</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>미설정 시 운영수동 차단</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>Branch Protection</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr">
+        <is>
+          <t>mvp-demo-verify 실패 시 merge가 막히는가?</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/branch_protection_check.txt</t>
+        </is>
+      </c>
       <c r="H12" s="2" t="n"/>
     </row>
     <row r="13">
@@ -13708,59 +14239,199 @@
       <c r="F9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>Normal answer + citation stream</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>정상 흐름에 citation(근거 인용) 이벤트가 포함되는가?</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>heartbeat→tool→citation→token→done 순서 확인</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/sse_stream_normal.log</t>
+        </is>
+      </c>
+      <c r="E10" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>PostgreSQL/Flyway boot</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>PG16.12 부팅과 마이그레이션이 정상 완료되는가?</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Database/Flyway/Tomcat started 마커 확인</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/backend_bootrun_postgres_output.txt</t>
+        </is>
+      </c>
+      <c r="E11" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="n"/>
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>SSE resume replay</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>last_event_id 이후 이벤트가 재생되는가?</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>id=3 이후 재생 + done 도달 확인</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/sse_resume_proof.log</t>
+        </is>
+      </c>
+      <c r="E12" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>SSE 실한도 검증</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>운영 한도(limit=2)에서도 3번째 연결이 429인가?</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>3번째 stream이 API-008-429-SSE로 차단</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/sse_concurrency_real_limit_proof.txt</t>
+        </is>
+      </c>
+      <c r="E13" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>아티팩트 보안 스캔</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>증빙 파일에 토큰/PII 원문이 없는가?</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>scan PASS + 검출건 0</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/artifact_sanitization_scan.txt</t>
+        </is>
+      </c>
+      <c r="E14" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="n"/>
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>문서 SSOT 정합성</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>00/03/04/06/PHASE2 상태표가 일치하는가?</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>consistency 게이트 PASS</t>
+        </is>
+      </c>
+      <c r="D15" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/e2e_runner_stdout.txt</t>
+        </is>
+      </c>
+      <c r="E15" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
-      <c r="E16" s="2" t="n"/>
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>브랜치 보호 설정</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>필수 체크 미통과 시 머지가 차단되는가?</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>required check가 등록됨</t>
+        </is>
+      </c>
+      <c r="D16" s="7" t="inlineStr">
+        <is>
+          <t>artifacts/branch_protection_check.txt</t>
+        </is>
+      </c>
+      <c r="E16" s="17" t="inlineStr">
+        <is>
+          <t>□</t>
+        </is>
+      </c>
       <c r="F16" s="2" t="n"/>
     </row>
     <row r="17">
@@ -15401,4 +16072,496 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="90" customWidth="1" min="2" max="2"/>
+    <col width="34" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="34" customHeight="1">
+      <c r="A1" s="18" t="inlineStr">
+        <is>
+          <t>CS 지원 AI 챗봇 - 경영진 보고용 1페이지 요약</t>
+        </is>
+      </c>
+      <c r="B1" s="19" t="n"/>
+      <c r="C1" s="20" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="21" t="inlineStr">
+        <is>
+          <t>작성 시각</t>
+        </is>
+      </c>
+      <c r="B2" s="22" t="inlineStr">
+        <is>
+          <t>2026-02-18 20:03</t>
+        </is>
+      </c>
+      <c r="C2" s="22" t="inlineStr">
+        <is>
+          <t>자동 생성</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="21" t="inlineStr">
+        <is>
+          <t>현재 단계</t>
+        </is>
+      </c>
+      <c r="B3" s="22" t="inlineStr">
+        <is>
+          <t>MVP Demo Ready 유지 + Phase2.1 운영 게이트 잠금 완료</t>
+        </is>
+      </c>
+      <c r="C3" s="22" t="inlineStr">
+        <is>
+          <t>진행중</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="21" t="inlineStr">
+        <is>
+          <t>핵심 결론</t>
+        </is>
+      </c>
+      <c r="B4" s="22" t="inlineStr">
+        <is>
+          <t>핵심 안전원칙(Fail-Closed/PII/trace/tenant)을 유지하면서, 문서-증빙-CI 게이트를 일치시키는 운영 잠금(Phase2.1)을 완료했습니다.</t>
+        </is>
+      </c>
+      <c r="C4" s="22" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="23" t="inlineStr"/>
+      <c r="B5" s="23" t="inlineStr"/>
+      <c r="C5" s="23" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="24" t="inlineStr">
+        <is>
+          <t>[이번 스프린트 핵심 성과]</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="n"/>
+      <c r="C6" s="20" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="23" t="inlineStr">
+        <is>
+          <t>1) 검증 자동화</t>
+        </is>
+      </c>
+      <c r="B7" s="23" t="inlineStr">
+        <is>
+          <t>CI/로컬 verify_all에서 SSOT consistency + 아티팩트 스캔 게이트를 강제했습니다.</t>
+        </is>
+      </c>
+      <c r="C7" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="23" t="inlineStr">
+        <is>
+          <t>2) 문서 단일화</t>
+        </is>
+      </c>
+      <c r="B8" s="23" t="inlineStr">
+        <is>
+          <t>검증 문서(00/03/04/06/PHASE2/CHANGELOG) 상태 매트릭스를 동일 기준으로 정렬했습니다.</t>
+        </is>
+      </c>
+      <c r="C8" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="23" t="inlineStr">
+        <is>
+          <t>3) 멱등성 고도화</t>
+        </is>
+      </c>
+      <c r="B9" s="23" t="inlineStr">
+        <is>
+          <t>Redis idempotency 전략을 운영/데모 환경별로 분리해 리스크를 명시했습니다.</t>
+        </is>
+      </c>
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="23" t="inlineStr">
+        <is>
+          <t>4) SSE 회귀 확장</t>
+        </is>
+      </c>
+      <c r="B10" s="23" t="inlineStr">
+        <is>
+          <t>SSE 동시성은 강제모드(limit=0) + 운영모드(limit=2) 2가지 시나리오로 증빙했습니다.</t>
+        </is>
+      </c>
+      <c r="C10" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="23" t="inlineStr">
+        <is>
+          <t>5) 관측 리포트</t>
+        </is>
+      </c>
+      <c r="B11" s="23" t="inlineStr">
+        <is>
+          <t>first-token/fail-closed/citation 지표를 자동 리포트하고 샘플수(n) 경고를 표시합니다.</t>
+        </is>
+      </c>
+      <c r="C11" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="23" t="inlineStr">
+        <is>
+          <t>6) 실제 Provider 회귀</t>
+        </is>
+      </c>
+      <c r="B12" s="23" t="inlineStr">
+        <is>
+          <t>Provider 회귀는 조용한 SKIPPED를 금지하고, 실행 가이드를 로그에 강제 출력합니다.</t>
+        </is>
+      </c>
+      <c r="C12" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="23" t="inlineStr"/>
+      <c r="B13" s="23" t="inlineStr"/>
+      <c r="C13" s="23" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="24" t="inlineStr">
+        <is>
+          <t>[핵심 운영 지표 - 최신 실행]</t>
+        </is>
+      </c>
+      <c r="B14" s="19" t="n"/>
+      <c r="C14" s="20" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="23" t="inlineStr">
+        <is>
+          <t>SSE 첫 토큰 지연 P50</t>
+        </is>
+      </c>
+      <c r="B15" s="27" t="inlineStr">
+        <is>
+          <t>0.983 ms</t>
+        </is>
+      </c>
+      <c r="C15" s="23" t="inlineStr">
+        <is>
+          <t>metrics_report.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="23" t="inlineStr">
+        <is>
+          <t>SSE 첫 토큰 지연 P95</t>
+        </is>
+      </c>
+      <c r="B16" s="27" t="inlineStr">
+        <is>
+          <t>1.999 ms</t>
+        </is>
+      </c>
+      <c r="C16" s="23" t="inlineStr">
+        <is>
+          <t>metrics_report.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="23" t="inlineStr">
+        <is>
+          <t>Fail-Closed 비율</t>
+        </is>
+      </c>
+      <c r="B17" s="27" t="inlineStr">
+        <is>
+          <t>0.047619047619047616</t>
+        </is>
+      </c>
+      <c r="C17" s="23" t="inlineStr">
+        <is>
+          <t>metrics_report.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="23" t="inlineStr">
+        <is>
+          <t>Citation Coverage</t>
+        </is>
+      </c>
+      <c r="B18" s="27" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C18" s="23" t="inlineStr">
+        <is>
+          <t>metrics_report.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="23" t="inlineStr">
+        <is>
+          <t>표본 수(n)</t>
+        </is>
+      </c>
+      <c r="B19" s="27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" s="23" t="inlineStr">
+        <is>
+          <t>metrics_report.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="24" t="inlineStr">
+        <is>
+          <t>[안전성 검증 체크]</t>
+        </is>
+      </c>
+      <c r="B20" s="19" t="n"/>
+      <c r="C20" s="20" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="23" t="inlineStr">
+        <is>
+          <t>정상 SSE 흐름</t>
+        </is>
+      </c>
+      <c r="B21" s="23" t="inlineStr">
+        <is>
+          <t>heartbeat -&gt; tool -&gt; citation -&gt; token -&gt; done</t>
+        </is>
+      </c>
+      <c r="C21" s="23" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="23" t="inlineStr">
+        <is>
+          <t>Fail-Closed 누출 방지</t>
+        </is>
+      </c>
+      <c r="B22" s="23" t="inlineStr">
+        <is>
+          <t>safe_response 후 done, answer token 누출 없음</t>
+        </is>
+      </c>
+      <c r="C22" s="23" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="23" t="inlineStr">
+        <is>
+          <t>Redis 멱등성(재시작 후)</t>
+        </is>
+      </c>
+      <c r="B23" s="23" t="inlineStr">
+        <is>
+          <t>첫 요청 201, 재요청 409(API-003-409)</t>
+        </is>
+      </c>
+      <c r="C23" s="23" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="23" t="inlineStr">
+        <is>
+          <t>Provider 회귀</t>
+        </is>
+      </c>
+      <c r="B24" s="23" t="inlineStr">
+        <is>
+          <t>환경 미설정 시 SKIPPED, 설정 시 PASS/FAIL 판정</t>
+        </is>
+      </c>
+      <c r="C24" s="23" t="inlineStr">
+        <is>
+          <t>SKIPPED(환경 미구성)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="23" t="inlineStr"/>
+      <c r="B25" s="23" t="inlineStr"/>
+      <c r="C25" s="23" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="23" t="inlineStr">
+        <is>
+          <t>[Phase2.1 잠금 결과]</t>
+        </is>
+      </c>
+      <c r="B26" s="19" t="n"/>
+      <c r="C26" s="20" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="23" t="inlineStr">
+        <is>
+          <t>브랜치 보호</t>
+        </is>
+      </c>
+      <c r="B27" s="23" t="inlineStr">
+        <is>
+          <t>문서+검증 스크립트 준비 완료(저장소 설정만 적용 필요)</t>
+        </is>
+      </c>
+      <c r="C27" s="23" t="inlineStr">
+        <is>
+          <t>진행중</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="23" t="inlineStr">
+        <is>
+          <t>문서 SSOT</t>
+        </is>
+      </c>
+      <c r="B28" s="23" t="inlineStr">
+        <is>
+          <t>00/03/04/06/PHASE2/CHANGELOG 정합성 게이트 PASS</t>
+        </is>
+      </c>
+      <c r="C28" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="23" t="inlineStr">
+        <is>
+          <t>아티팩트 보안</t>
+        </is>
+      </c>
+      <c r="B29" s="23" t="inlineStr">
+        <is>
+          <t>민감정보 스캔 PASS (검출 0건)</t>
+        </is>
+      </c>
+      <c r="C29" s="23" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B30" s="28" t="inlineStr">
+        <is>
+          <t>로컬 Node 버전(24)과 프론트 요구 버전(22) 불일치 경고가 존재합니다.</t>
+        </is>
+      </c>
+      <c r="C30" s="23" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B31" s="28" t="inlineStr">
+        <is>
+          <t>sse_first_token 지표는 표본 수가 작아 통계 안정성 보강이 필요합니다.</t>
+        </is>
+      </c>
+      <c r="C31" s="23" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="23" t="inlineStr"/>
+      <c r="B32" s="23" t="inlineStr"/>
+      <c r="C32" s="23" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="23" t="inlineStr">
+        <is>
+          <t>참조 문서</t>
+        </is>
+      </c>
+      <c r="B33" s="23" t="inlineStr">
+        <is>
+          <t>PHASE2_PROGRESS_SUMMARY_FOR_CHATGPT.md</t>
+        </is>
+      </c>
+      <c r="C33" s="23" t="inlineStr">
+        <is>
+          <t>최상단</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A20:C20"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: finalize phase2 auth rbac ops hardening and reports
</commit_message>
<xml_diff>
--- a/07_MVP_GLOSSARY_CEO_KR.xlsx
+++ b/07_MVP_GLOSSARY_CEO_KR.xlsx
@@ -14,7 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="경영진1페이지요약" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'용어사전'!$A$4:$J$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'용어사전'!$A$4:$J$79</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -2330,647 +2330,2487 @@
       <c r="K33" s="2" t="n"/>
       <c r="L33" s="2" t="n"/>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n"/>
-      <c r="B34" s="2" t="n"/>
-      <c r="C34" s="2" t="n"/>
-      <c r="D34" s="2" t="n"/>
-      <c r="E34" s="2" t="n"/>
-      <c r="F34" s="2" t="n"/>
-      <c r="G34" s="2" t="n"/>
-      <c r="H34" s="2" t="n"/>
-      <c r="I34" s="2" t="n"/>
-      <c r="J34" s="2" t="n"/>
+    <row r="34" ht="68" customHeight="1">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>Contextual Retrieval</t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ?? ?? ???? ??? ??</t>
+        </is>
+      </c>
+      <c r="D34" s="7" t="inlineStr">
+        <is>
+          <t>RAG RetrievalService, ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="inlineStr">
+        <is>
+          <t>?? ????? ?? ??? ?? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t>'? ??? ????' ??? ?? ?? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="G34" s="7" t="inlineStr">
+        <is>
+          <t>?? ????? ???? ??? ??? ??? ?? ? ??</t>
+        </is>
+      </c>
+      <c r="H34" s="7" t="inlineStr">
+        <is>
+          <t>rag_search_ms, zero_evidence_rate</t>
+        </is>
+      </c>
+      <c r="I34" s="7" t="inlineStr">
+        <is>
+          <t>?? ??? ??/?? ?? 2? ??</t>
+        </is>
+      </c>
+      <c r="J34" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K34" s="2" t="n"/>
       <c r="L34" s="2" t="n"/>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n"/>
-      <c r="B35" s="2" t="n"/>
-      <c r="C35" s="2" t="n"/>
-      <c r="D35" s="2" t="n"/>
-      <c r="E35" s="2" t="n"/>
-      <c r="F35" s="2" t="n"/>
-      <c r="G35" s="2" t="n"/>
-      <c r="H35" s="2" t="n"/>
-      <c r="I35" s="2" t="n"/>
-      <c r="J35" s="2" t="n"/>
+    <row r="35" ht="68" customHeight="1">
+      <c r="A35" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B35" s="9" t="inlineStr">
+        <is>
+          <t>Summary-first Retrieval</t>
+        </is>
+      </c>
+      <c r="C35" s="9" t="inlineStr">
+        <is>
+          <t>?? ???? ?? ???? ?? ??? ??? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="D35" s="9" t="inlineStr">
+        <is>
+          <t>RAG ?? ???, chunk summary ??</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ???? ?? ??? ?? ?? ?</t>
+        </is>
+      </c>
+      <c r="F35" s="9" t="inlineStr">
+        <is>
+          <t>? ?? ???? ?? ??? ?? ?? ???? ???</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ??? ??? ??? ?? ??? ? ??</t>
+        </is>
+      </c>
+      <c r="H35" s="9" t="inlineStr">
+        <is>
+          <t>first_token_ms, rag_search_ms</t>
+        </is>
+      </c>
+      <c r="I35" s="9" t="inlineStr">
+        <is>
+          <t>?? on/off ???? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="J35" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K35" s="2" t="n"/>
       <c r="L35" s="2" t="n"/>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n"/>
-      <c r="B36" s="2" t="n"/>
-      <c r="C36" s="2" t="n"/>
-      <c r="D36" s="2" t="n"/>
-      <c r="E36" s="2" t="n"/>
-      <c r="F36" s="2" t="n"/>
-      <c r="G36" s="2" t="n"/>
-      <c r="H36" s="2" t="n"/>
-      <c r="I36" s="2" t="n"/>
-      <c r="J36" s="2" t="n"/>
+    <row r="36" ht="68" customHeight="1">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="inlineStr">
+        <is>
+          <t>Hybrid Search</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ??? ??? ?? ?? ?? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t>RetrievalService, RAG ?????</t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ??? ???? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="F36" s="5" t="inlineStr">
+        <is>
+          <t>???? ??, ?? ??? ???? ??? ??</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ???? ?? ???? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H36" s="5" t="inlineStr">
+        <is>
+          <t>bm25_ms, vector_ms, rrf_ms</t>
+        </is>
+      </c>
+      <c r="I36" s="5" t="inlineStr">
+        <is>
+          <t>??? ??? ?? ??? ??? ?? ???</t>
+        </is>
+      </c>
+      <c r="J36" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K36" s="2" t="n"/>
       <c r="L36" s="2" t="n"/>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n"/>
-      <c r="B37" s="2" t="n"/>
-      <c r="C37" s="2" t="n"/>
-      <c r="D37" s="2" t="n"/>
-      <c r="E37" s="2" t="n"/>
-      <c r="F37" s="2" t="n"/>
-      <c r="G37" s="2" t="n"/>
-      <c r="H37" s="2" t="n"/>
-      <c r="I37" s="2" t="n"/>
-      <c r="J37" s="2" t="n"/>
+    <row r="37" ht="68" customHeight="1">
+      <c r="A37" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B37" s="7" t="inlineStr">
+        <is>
+          <t>BM25</t>
+        </is>
+      </c>
+      <c r="C37" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ??? ????? ?? ?? ????</t>
+        </is>
+      </c>
+      <c r="D37" s="7" t="inlineStr">
+        <is>
+          <t>Hybrid Search? ??? ?</t>
+        </is>
+      </c>
+      <c r="E37" s="7" t="inlineStr">
+        <is>
+          <t>??? ???/?? ???? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="F37" s="7" t="inlineStr">
+        <is>
+          <t>'API-008' ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G37" s="7" t="inlineStr">
+        <is>
+          <t>???/??? ?? ??? ?? ?? ??? ?</t>
+        </is>
+      </c>
+      <c r="H37" s="7" t="inlineStr">
+        <is>
+          <t>bm25_ms, citation_count</t>
+        </is>
+      </c>
+      <c r="I37" s="7" t="inlineStr">
+        <is>
+          <t>?? ??/?? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J37" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K37" s="2" t="n"/>
       <c r="L37" s="2" t="n"/>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n"/>
-      <c r="B38" s="2" t="n"/>
-      <c r="C38" s="2" t="n"/>
-      <c r="D38" s="2" t="n"/>
-      <c r="E38" s="2" t="n"/>
-      <c r="F38" s="2" t="n"/>
-      <c r="G38" s="2" t="n"/>
-      <c r="H38" s="2" t="n"/>
-      <c r="I38" s="2" t="n"/>
-      <c r="J38" s="2" t="n"/>
+    <row r="38" ht="68" customHeight="1">
+      <c r="A38" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B38" s="9" t="inlineStr">
+        <is>
+          <t>RRF</t>
+        </is>
+      </c>
+      <c r="C38" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ??? ?? ?? ??? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="D38" s="9" t="inlineStr">
+        <is>
+          <t>RrfFusion, RetrievalService</t>
+        </is>
+      </c>
+      <c r="E38" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="F38" s="9" t="inlineStr">
+        <is>
+          <t>?? 1?? BM25 1?? ?? ??? ?? Top-K ??</t>
+        </is>
+      </c>
+      <c r="G38" s="9" t="inlineStr">
+        <is>
+          <t>k ? ??? ??? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H38" s="9" t="inlineStr">
+        <is>
+          <t>rrf_ms, zero_evidence_rate</t>
+        </is>
+      </c>
+      <c r="I38" s="9" t="inlineStr">
+        <is>
+          <t>RRF on/off ? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="J38" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K38" s="2" t="n"/>
       <c r="L38" s="2" t="n"/>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n"/>
-      <c r="B39" s="2" t="n"/>
-      <c r="C39" s="2" t="n"/>
-      <c r="D39" s="2" t="n"/>
-      <c r="E39" s="2" t="n"/>
-      <c r="F39" s="2" t="n"/>
-      <c r="G39" s="2" t="n"/>
-      <c r="H39" s="2" t="n"/>
-      <c r="I39" s="2" t="n"/>
-      <c r="J39" s="2" t="n"/>
+    <row r="39" ht="68" customHeight="1">
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <t>Reranker</t>
+        </is>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
+        <is>
+          <t>1? ?? ??? 2?? ???? ?? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="D39" s="7" t="inlineStr">
+        <is>
+          <t>RetrievalService rerank ??</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ?? fail-closed ??? ???</t>
+        </is>
+      </c>
+      <c r="F39" s="7" t="inlineStr">
+        <is>
+          <t>Top-20 ??? ???? ?? Top-5 ??</t>
+        </is>
+      </c>
+      <c r="G39" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ??? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H39" s="7" t="inlineStr">
+        <is>
+          <t>rerank_ms, citation_click_rate</t>
+        </is>
+      </c>
+      <c r="I39" s="7" t="inlineStr">
+        <is>
+          <t>rerank on/off ? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J39" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K39" s="2" t="n"/>
       <c r="L39" s="2" t="n"/>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n"/>
-      <c r="B40" s="2" t="n"/>
-      <c r="C40" s="2" t="n"/>
-      <c r="D40" s="2" t="n"/>
-      <c r="E40" s="2" t="n"/>
-      <c r="F40" s="2" t="n"/>
-      <c r="G40" s="2" t="n"/>
-      <c r="H40" s="2" t="n"/>
-      <c r="I40" s="2" t="n"/>
-      <c r="J40" s="2" t="n"/>
+    <row r="40" ht="68" customHeight="1">
+      <c r="A40" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B40" s="9" t="inlineStr">
+        <is>
+          <t>NoopReranker</t>
+        </is>
+      </c>
+      <c r="C40" s="9" t="inlineStr">
+        <is>
+          <t>????? ?? ??? ??? ? ???? ??? ????? ??</t>
+        </is>
+      </c>
+      <c r="D40" s="9" t="inlineStr">
+        <is>
+          <t>RAG ??/?? ????</t>
+        </is>
+      </c>
+      <c r="E40" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ? ?? reranker ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F40" s="9" t="inlineStr">
+        <is>
+          <t>?? ???? ??? ??? ????? ??? ??</t>
+        </is>
+      </c>
+      <c r="G40" s="9" t="inlineStr">
+        <is>
+          <t>???? ??? ?? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="H40" s="9" t="inlineStr">
+        <is>
+          <t>rerank_ms, fail_closed_count</t>
+        </is>
+      </c>
+      <c r="I40" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="J40" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K40" s="2" t="n"/>
       <c r="L40" s="2" t="n"/>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n"/>
-      <c r="B41" s="2" t="n"/>
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" s="2" t="n"/>
-      <c r="E41" s="2" t="n"/>
-      <c r="F41" s="2" t="n"/>
-      <c r="G41" s="2" t="n"/>
-      <c r="H41" s="2" t="n"/>
-      <c r="I41" s="2" t="n"/>
-      <c r="J41" s="2" t="n"/>
+    <row r="41" ht="68" customHeight="1">
+      <c r="A41" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B41" s="7" t="inlineStr">
+        <is>
+          <t>ExtractiveChunkSummarizer</t>
+        </is>
+      </c>
+      <c r="C41" s="7" t="inlineStr">
+        <is>
+          <t>???? ?? ??? ??? ?? ??? ??? ????</t>
+        </is>
+      </c>
+      <c r="D41" s="7" t="inlineStr">
+        <is>
+          <t>RAG ??/???? ??</t>
+        </is>
+      </c>
+      <c r="E41" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F41" s="7" t="inlineStr">
+        <is>
+          <t>? ?? ???? ?? ?? 2~3??? ??</t>
+        </is>
+      </c>
+      <c r="G41" s="7" t="inlineStr">
+        <is>
+          <t>?? ???? ?? ?? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H41" s="7" t="inlineStr">
+        <is>
+          <t>token_usage, citation_coverage</t>
+        </is>
+      </c>
+      <c r="I41" s="7" t="inlineStr">
+        <is>
+          <t>???? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="J41" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K41" s="2" t="n"/>
       <c r="L41" s="2" t="n"/>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n"/>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="2" t="n"/>
-      <c r="F42" s="2" t="n"/>
-      <c r="G42" s="2" t="n"/>
-      <c r="H42" s="2" t="n"/>
-      <c r="I42" s="2" t="n"/>
-      <c r="J42" s="2" t="n"/>
+    <row r="42" ht="68" customHeight="1">
+      <c r="A42" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B42" s="9" t="inlineStr">
+        <is>
+          <t>top_k</t>
+        </is>
+      </c>
+      <c r="C42" s="9" t="inlineStr">
+        <is>
+          <t>?? ???? ????? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="D42" s="9" t="inlineStr">
+        <is>
+          <t>RAG API ??/?? ??</t>
+        </is>
+      </c>
+      <c r="E42" s="9" t="inlineStr">
+        <is>
+          <t>?????????? ??? ???? ?? ????</t>
+        </is>
+      </c>
+      <c r="F42" s="9" t="inlineStr">
+        <is>
+          <t>top_k=5? ???? ?? ??, top_k=20? ?? ??</t>
+        </is>
+      </c>
+      <c r="G42" s="9" t="inlineStr">
+        <is>
+          <t>???? ??? ??/?? ???? ???</t>
+        </is>
+      </c>
+      <c r="H42" s="9" t="inlineStr">
+        <is>
+          <t>topk_guard_trigger_count, API-008-429-BUDGET</t>
+        </is>
+      </c>
+      <c r="I42" s="9" t="inlineStr">
+        <is>
+          <t>top_k 5/10/20 ?? ??</t>
+        </is>
+      </c>
+      <c r="J42" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K42" s="2" t="n"/>
       <c r="L42" s="2" t="n"/>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n"/>
-      <c r="B43" s="2" t="n"/>
-      <c r="C43" s="2" t="n"/>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="2" t="n"/>
-      <c r="F43" s="2" t="n"/>
-      <c r="G43" s="2" t="n"/>
-      <c r="H43" s="2" t="n"/>
-      <c r="I43" s="2" t="n"/>
-      <c r="J43" s="2" t="n"/>
+    <row r="43" ht="68" customHeight="1">
+      <c r="A43" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="inlineStr">
+        <is>
+          <t>chunk_id</t>
+        </is>
+      </c>
+      <c r="C43" s="7" t="inlineStr">
+        <is>
+          <t>??? ? ?? ??? ?? ???</t>
+        </is>
+      </c>
+      <c r="D43" s="7" t="inlineStr">
+        <is>
+          <t>Citation ??/??, Answer Contract</t>
+        </is>
+      </c>
+      <c r="E43" s="7" t="inlineStr">
+        <is>
+          <t>?? ? '?? ?????'? ??? ? ??</t>
+        </is>
+      </c>
+      <c r="F43" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ???? chunk_id? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G43" s="7" t="inlineStr">
+        <is>
+          <t>chunk_id ?? ???? ???? ???? ???</t>
+        </is>
+      </c>
+      <c r="H43" s="7" t="inlineStr">
+        <is>
+          <t>AI-009-409-CITATION</t>
+        </is>
+      </c>
+      <c r="I43" s="7" t="inlineStr">
+        <is>
+          <t>??? citation? chunk_id ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J43" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K43" s="2" t="n"/>
       <c r="L43" s="2" t="n"/>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n"/>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="2" t="n"/>
-      <c r="E44" s="2" t="n"/>
-      <c r="F44" s="2" t="n"/>
-      <c r="G44" s="2" t="n"/>
-      <c r="H44" s="2" t="n"/>
-      <c r="I44" s="2" t="n"/>
-      <c r="J44" s="2" t="n"/>
+    <row r="44" ht="68" customHeight="1">
+      <c r="A44" s="5" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="inlineStr">
+        <is>
+          <t>MyBatis</t>
+        </is>
+      </c>
+      <c r="C44" s="5" t="inlineStr">
+        <is>
+          <t>Mapper ?????? XML? DB ??? ???? ?????</t>
+        </is>
+      </c>
+      <c r="D44" s="5" t="inlineStr">
+        <is>
+          <t>backend mappers, repository</t>
+        </is>
+      </c>
+      <c r="E44" s="5" t="inlineStr">
+        <is>
+          <t>SQL ??? ?? ??(tenant_key ?) ??? ??</t>
+        </is>
+      </c>
+      <c r="F44" s="5" t="inlineStr">
+        <is>
+          <t>Repository? Mapper? ???? ??/??</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>?? JDBC ?? ? ?? ??/?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H44" s="5" t="inlineStr">
+        <is>
+          <t>mybatis_dollar_scan_output.txt</t>
+        </is>
+      </c>
+      <c r="I44" s="5" t="inlineStr">
+        <is>
+          <t>Mapper ?? ??? `${}` 0? ??</t>
+        </is>
+      </c>
+      <c r="J44" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K44" s="2" t="n"/>
       <c r="L44" s="2" t="n"/>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n"/>
-      <c r="B45" s="2" t="n"/>
-      <c r="C45" s="2" t="n"/>
-      <c r="D45" s="2" t="n"/>
-      <c r="E45" s="2" t="n"/>
-      <c r="F45" s="2" t="n"/>
-      <c r="G45" s="2" t="n"/>
-      <c r="H45" s="2" t="n"/>
-      <c r="I45" s="2" t="n"/>
-      <c r="J45" s="2" t="n"/>
+    <row r="45" ht="68" customHeight="1">
+      <c r="A45" s="9" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B45" s="9" t="inlineStr">
+        <is>
+          <t>resultMap</t>
+        </is>
+      </c>
+      <c r="C45" s="9" t="inlineStr">
+        <is>
+          <t>DB ??? ?? ?? ??? ????? ???? MyBatis ??</t>
+        </is>
+      </c>
+      <c r="D45" s="9" t="inlineStr">
+        <is>
+          <t>*Mapper.xml</t>
+        </is>
+      </c>
+      <c r="E45" s="9" t="inlineStr">
+        <is>
+          <t>?? ????? ?? ??? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F45" s="9" t="inlineStr">
+        <is>
+          <t>chunk_id -&gt; chunkId, created_at -&gt; createdAt ??</t>
+        </is>
+      </c>
+      <c r="G45" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="H45" s="9" t="inlineStr">
+        <is>
+          <t>mapper mapping contract</t>
+        </is>
+      </c>
+      <c r="I45" s="9" t="inlineStr">
+        <is>
+          <t>?? Mapper XML? resultMap ?? ??</t>
+        </is>
+      </c>
+      <c r="J45" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K45" s="2" t="n"/>
       <c r="L45" s="2" t="n"/>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n"/>
-      <c r="B46" s="2" t="n"/>
-      <c r="C46" s="2" t="n"/>
-      <c r="D46" s="2" t="n"/>
-      <c r="E46" s="2" t="n"/>
-      <c r="F46" s="2" t="n"/>
-      <c r="G46" s="2" t="n"/>
-      <c r="H46" s="2" t="n"/>
-      <c r="I46" s="2" t="n"/>
-      <c r="J46" s="2" t="n"/>
+    <row r="46" ht="68" customHeight="1">
+      <c r="A46" s="7" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B46" s="7" t="inlineStr">
+        <is>
+          <t>UUIDTypeHandler</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>UUID ??? DB? ?? ???? ???? ???? MyBatis ???</t>
+        </is>
+      </c>
+      <c r="D46" s="7" t="inlineStr">
+        <is>
+          <t>global/mybatis/UUIDTypeHandler</t>
+        </is>
+      </c>
+      <c r="E46" s="7" t="inlineStr">
+        <is>
+          <t>uuid ?? ?? ??? ????? ??</t>
+        </is>
+      </c>
+      <c r="F46" s="7" t="inlineStr">
+        <is>
+          <t>String ??? ?? UUID ???? ???</t>
+        </is>
+      </c>
+      <c r="G46" s="7" t="inlineStr">
+        <is>
+          <t>??? ??? ? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H46" s="7" t="inlineStr">
+        <is>
+          <t>uuid_cast_scan_output.txt</t>
+        </is>
+      </c>
+      <c r="I46" s="7" t="inlineStr">
+        <is>
+          <t>UUID ?? Mapper ?? ?? ???</t>
+        </is>
+      </c>
+      <c r="J46" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K46" s="2" t="n"/>
       <c r="L46" s="2" t="n"/>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n"/>
-      <c r="B47" s="2" t="n"/>
-      <c r="C47" s="2" t="n"/>
-      <c r="D47" s="2" t="n"/>
-      <c r="E47" s="2" t="n"/>
-      <c r="F47" s="2" t="n"/>
-      <c r="G47" s="2" t="n"/>
-      <c r="H47" s="2" t="n"/>
-      <c r="I47" s="2" t="n"/>
-      <c r="J47" s="2" t="n"/>
+    <row r="47" ht="68" customHeight="1">
+      <c r="A47" s="9" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B47" s="9" t="inlineStr">
+        <is>
+          <t>TypeHandler</t>
+        </is>
+      </c>
+      <c r="C47" s="9" t="inlineStr">
+        <is>
+          <t>MyBatis?? ??? ?? ?? ?? ??? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="D47" s="9" t="inlineStr">
+        <is>
+          <t>MyBatis ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="E47" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ? ??? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="F47" s="9" t="inlineStr">
+        <is>
+          <t>UUID, JSON ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="inlineStr">
+        <is>
+          <t>???? ?? ?? ?? ? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H47" s="9" t="inlineStr">
+        <is>
+          <t>mapper bind error rate</t>
+        </is>
+      </c>
+      <c r="I47" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="J47" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K47" s="2" t="n"/>
       <c r="L47" s="2" t="n"/>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n"/>
-      <c r="B48" s="2" t="n"/>
-      <c r="C48" s="2" t="n"/>
-      <c r="D48" s="2" t="n"/>
-      <c r="E48" s="2" t="n"/>
-      <c r="F48" s="2" t="n"/>
-      <c r="G48" s="2" t="n"/>
-      <c r="H48" s="2" t="n"/>
-      <c r="I48" s="2" t="n"/>
-      <c r="J48" s="2" t="n"/>
+    <row r="48" ht="68" customHeight="1">
+      <c r="A48" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="inlineStr">
+        <is>
+          <t>client_nonce</t>
+        </is>
+      </c>
+      <c r="C48" s="7" t="inlineStr">
+        <is>
+          <t>?????? ?? ???? ???? ?? ?</t>
+        </is>
+      </c>
+      <c r="D48" s="7" t="inlineStr">
+        <is>
+          <t>??/??? ?? API</t>
+        </is>
+      </c>
+      <c r="E48" s="7" t="inlineStr">
+        <is>
+          <t>?? ??/????? ?? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F48" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ? ?? nonce? ?? ??</t>
+        </is>
+      </c>
+      <c r="G48" s="7" t="inlineStr">
+        <is>
+          <t>nonce ??? ??? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H48" s="7" t="inlineStr">
+        <is>
+          <t>API-003-409, API-003-422</t>
+        </is>
+      </c>
+      <c r="I48" s="7" t="inlineStr">
+        <is>
+          <t>?? nonce? 2? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J48" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K48" s="2" t="n"/>
       <c r="L48" s="2" t="n"/>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n"/>
-      <c r="B49" s="2" t="n"/>
-      <c r="C49" s="2" t="n"/>
-      <c r="D49" s="2" t="n"/>
-      <c r="E49" s="2" t="n"/>
-      <c r="F49" s="2" t="n"/>
-      <c r="G49" s="2" t="n"/>
-      <c r="H49" s="2" t="n"/>
-      <c r="I49" s="2" t="n"/>
-      <c r="J49" s="2" t="n"/>
+    <row r="49" ht="68" customHeight="1">
+      <c r="A49" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B49" s="9" t="inlineStr">
+        <is>
+          <t>payload_hash</t>
+        </is>
+      </c>
+      <c r="C49" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ??? ??? ?? ?? ???? ?</t>
+        </is>
+      </c>
+      <c r="D49" s="9" t="inlineStr">
+        <is>
+          <t>IdempotencyService, RedisIdempotencyStore</t>
+        </is>
+      </c>
+      <c r="E49" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ??? ???? ??/?? ?? ??</t>
+        </is>
+      </c>
+      <c r="F49" s="9" t="inlineStr">
+        <is>
+          <t>Idempotency-Key ??, body ?? -&gt; ??</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ??? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H49" s="9" t="inlineStr">
+        <is>
+          <t>idempotency_negative_422.txt</t>
+        </is>
+      </c>
+      <c r="I49" s="9" t="inlineStr">
+        <is>
+          <t>?? ?+?? payload ?? ???</t>
+        </is>
+      </c>
+      <c r="J49" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K49" s="2" t="n"/>
       <c r="L49" s="2" t="n"/>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n"/>
-      <c r="B50" s="2" t="n"/>
-      <c r="C50" s="2" t="n"/>
-      <c r="D50" s="2" t="n"/>
-      <c r="E50" s="2" t="n"/>
-      <c r="F50" s="2" t="n"/>
-      <c r="G50" s="2" t="n"/>
-      <c r="H50" s="2" t="n"/>
-      <c r="I50" s="2" t="n"/>
-      <c r="J50" s="2" t="n"/>
+    <row r="50" ht="68" customHeight="1">
+      <c r="A50" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>RedisIdempotencyStore</t>
+        </is>
+      </c>
+      <c r="C50" s="7" t="inlineStr">
+        <is>
+          <t>?? ???? ??? ??? Redis? ???? ??</t>
+        </is>
+      </c>
+      <c r="D50" s="7" t="inlineStr">
+        <is>
+          <t>global/idempotency</t>
+        </is>
+      </c>
+      <c r="E50" s="7" t="inlineStr">
+        <is>
+          <t>?? ??????? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F50" s="7" t="inlineStr">
+        <is>
+          <t>?? 2? ????? ?? ?? 1? ??</t>
+        </is>
+      </c>
+      <c r="G50" s="7" t="inlineStr">
+        <is>
+          <t>Redis ?? ? fallback ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="H50" s="7" t="inlineStr">
+        <is>
+          <t>NEG-IDEM-REDIS-001</t>
+        </is>
+      </c>
+      <c r="I50" s="7" t="inlineStr">
+        <is>
+          <t>Redis on/off?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="J50" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K50" s="2" t="n"/>
       <c r="L50" s="2" t="n"/>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n"/>
-      <c r="B51" s="2" t="n"/>
-      <c r="C51" s="2" t="n"/>
-      <c r="D51" s="2" t="n"/>
-      <c r="E51" s="2" t="n"/>
-      <c r="F51" s="2" t="n"/>
-      <c r="G51" s="2" t="n"/>
-      <c r="H51" s="2" t="n"/>
-      <c r="I51" s="2" t="n"/>
-      <c r="J51" s="2" t="n"/>
+    <row r="51" ht="68" customHeight="1">
+      <c r="A51" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B51" s="9" t="inlineStr">
+        <is>
+          <t>RagIdempotencyRegistry</t>
+        </is>
+      </c>
+      <c r="C51" s="9" t="inlineStr">
+        <is>
+          <t>RAG ?? ?? ?? ?? ??? ???? ?????</t>
+        </is>
+      </c>
+      <c r="D51" s="9" t="inlineStr">
+        <is>
+          <t>RagController</t>
+        </is>
+      </c>
+      <c r="E51" s="9" t="inlineStr">
+        <is>
+          <t>RAG ??? ? ?? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F51" s="9" t="inlineStr">
+        <is>
+          <t>retrieve/answer ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="G51" s="9" t="inlineStr">
+        <is>
+          <t>?? ? ??? ???? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H51" s="9" t="inlineStr">
+        <is>
+          <t>API-003-409</t>
+        </is>
+      </c>
+      <c r="I51" s="9" t="inlineStr">
+        <is>
+          <t>?? ?/?? ? RAG ?? ??</t>
+        </is>
+      </c>
+      <c r="J51" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K51" s="2" t="n"/>
       <c r="L51" s="2" t="n"/>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n"/>
-      <c r="B52" s="2" t="n"/>
-      <c r="C52" s="2" t="n"/>
-      <c r="D52" s="2" t="n"/>
-      <c r="E52" s="2" t="n"/>
-      <c r="F52" s="2" t="n"/>
-      <c r="G52" s="2" t="n"/>
-      <c r="H52" s="2" t="n"/>
-      <c r="I52" s="2" t="n"/>
-      <c r="J52" s="2" t="n"/>
+    <row r="52" ht="68" customHeight="1">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>UUID CAST</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>SQL?? CAST(... AS UUID) ?? ??? ???? ?? ???</t>
+        </is>
+      </c>
+      <c r="D52" s="7" t="inlineStr">
+        <is>
+          <t>Mapper ?? ??, CI ???</t>
+        </is>
+      </c>
+      <c r="E52" s="7" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F52" s="7" t="inlineStr">
+        <is>
+          <t>?? Mapper?? CAST ?? ?? ? CI ??</t>
+        </is>
+      </c>
+      <c r="G52" s="7" t="inlineStr">
+        <is>
+          <t>?? ??? ???? ?? ???</t>
+        </is>
+      </c>
+      <c r="H52" s="7" t="inlineStr">
+        <is>
+          <t>uuid_cast_scan_output.txt</t>
+        </is>
+      </c>
+      <c r="I52" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? NO_MATCH ??</t>
+        </is>
+      </c>
+      <c r="J52" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K52" s="2" t="n"/>
       <c r="L52" s="2" t="n"/>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n"/>
-      <c r="B53" s="2" t="n"/>
-      <c r="C53" s="2" t="n"/>
-      <c r="D53" s="2" t="n"/>
-      <c r="E53" s="2" t="n"/>
-      <c r="F53" s="2" t="n"/>
-      <c r="G53" s="2" t="n"/>
-      <c r="H53" s="2" t="n"/>
-      <c r="I53" s="2" t="n"/>
-      <c r="J53" s="2" t="n"/>
+    <row r="53" ht="68" customHeight="1">
+      <c r="A53" s="5" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B53" s="5" t="inlineStr">
+        <is>
+          <t>tenant_key_mismatch</t>
+        </is>
+      </c>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>?? ???? ??/??? ???? ?? ? ???? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="D53" s="5" t="inlineStr">
+        <is>
+          <t>AuthService, Tenant filter</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ??? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="F53" s="5" t="inlineStr">
+        <is>
+          <t>A??? ???? B??? ??? ?? -&gt; 403</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>UI ?????? ?? ???, ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H53" s="5" t="inlineStr">
+        <is>
+          <t>SYS-002-403</t>
+        </is>
+      </c>
+      <c r="I53" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ???? E2E ??</t>
+        </is>
+      </c>
+      <c r="J53" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K53" s="2" t="n"/>
       <c r="L53" s="2" t="n"/>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n"/>
-      <c r="B54" s="2" t="n"/>
-      <c r="C54" s="2" t="n"/>
-      <c r="D54" s="2" t="n"/>
-      <c r="E54" s="2" t="n"/>
-      <c r="F54" s="2" t="n"/>
-      <c r="G54" s="2" t="n"/>
-      <c r="H54" s="2" t="n"/>
-      <c r="I54" s="2" t="n"/>
-      <c r="J54" s="2" t="n"/>
+    <row r="54" ht="68" customHeight="1">
+      <c r="A54" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B54" s="9" t="inlineStr">
+        <is>
+          <t>Last-Event-ID</t>
+        </is>
+      </c>
+      <c r="C54" s="9" t="inlineStr">
+        <is>
+          <t>?? SSE ???? ???? ?? ??? ??? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="D54" s="9" t="inlineStr">
+        <is>
+          <t>stream/resume API</t>
+        </is>
+      </c>
+      <c r="E54" s="9" t="inlineStr">
+        <is>
+          <t>???? ??? ???? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="F54" s="9" t="inlineStr">
+        <is>
+          <t>1~30? ?? ? ??, 31??? ??</t>
+        </is>
+      </c>
+      <c r="G54" s="9" t="inlineStr">
+        <is>
+          <t>??? ID ??/?? ?? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H54" s="9" t="inlineStr">
+        <is>
+          <t>SSE-RESUME-001</t>
+        </is>
+      </c>
+      <c r="I54" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ? resume ?? ??</t>
+        </is>
+      </c>
+      <c r="J54" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K54" s="2" t="n"/>
       <c r="L54" s="2" t="n"/>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n"/>
-      <c r="B55" s="2" t="n"/>
-      <c r="C55" s="2" t="n"/>
-      <c r="D55" s="2" t="n"/>
-      <c r="E55" s="2" t="n"/>
-      <c r="F55" s="2" t="n"/>
-      <c r="G55" s="2" t="n"/>
-      <c r="H55" s="2" t="n"/>
-      <c r="I55" s="2" t="n"/>
-      <c r="J55" s="2" t="n"/>
+    <row r="55" ht="68" customHeight="1">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="inlineStr">
+        <is>
+          <t>SSE resume</t>
+        </is>
+      </c>
+      <c r="C55" s="7" t="inlineStr">
+        <is>
+          <t>SSE ??? ??? ? ???? ?? ??? ????? ??</t>
+        </is>
+      </c>
+      <c r="D55" s="7" t="inlineStr">
+        <is>
+          <t>MessageStreamV1Controller /stream/resume</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>??? ???? ???? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F55" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ? ?? message_id? ??</t>
+        </is>
+      </c>
+      <c r="G55" s="7" t="inlineStr">
+        <is>
+          <t>resume ?? ? fallback ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="H55" s="7" t="inlineStr">
+        <is>
+          <t>SSE-RESUME-NET-001</t>
+        </is>
+      </c>
+      <c r="I55" s="7" t="inlineStr">
+        <is>
+          <t>fault injection ??? ??</t>
+        </is>
+      </c>
+      <c r="J55" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K55" s="2" t="n"/>
       <c r="L55" s="2" t="n"/>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n"/>
-      <c r="B56" s="2" t="n"/>
-      <c r="C56" s="2" t="n"/>
-      <c r="D56" s="2" t="n"/>
-      <c r="E56" s="2" t="n"/>
-      <c r="F56" s="2" t="n"/>
-      <c r="G56" s="2" t="n"/>
-      <c r="H56" s="2" t="n"/>
-      <c r="I56" s="2" t="n"/>
-      <c r="J56" s="2" t="n"/>
+    <row r="56" ht="68" customHeight="1">
+      <c r="A56" s="5" t="inlineStr">
+        <is>
+          <t>??/???</t>
+        </is>
+      </c>
+      <c r="B56" s="5" t="inlineStr">
+        <is>
+          <t>SseConcurrencyGuard</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>???? SSE ?? ?? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>message/application/SseConcurrencyGuard</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F56" s="5" t="inlineStr">
+        <is>
+          <t>3?? ?? ??? ??? 429? ??</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ? ?? ????? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H56" s="5" t="inlineStr">
+        <is>
+          <t>API-008-429-SSE</t>
+        </is>
+      </c>
+      <c r="I56" s="5" t="inlineStr">
+        <is>
+          <t>?? 3?? ???? ??</t>
+        </is>
+      </c>
+      <c r="J56" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K56" s="2" t="n"/>
       <c r="L56" s="2" t="n"/>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n"/>
-      <c r="B57" s="2" t="n"/>
-      <c r="C57" s="2" t="n"/>
-      <c r="D57" s="2" t="n"/>
-      <c r="E57" s="2" t="n"/>
-      <c r="F57" s="2" t="n"/>
-      <c r="G57" s="2" t="n"/>
-      <c r="H57" s="2" t="n"/>
-      <c r="I57" s="2" t="n"/>
-      <c r="J57" s="2" t="n"/>
+    <row r="57" ht="68" customHeight="1">
+      <c r="A57" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B57" s="9" t="inlineStr">
+        <is>
+          <t>Retry-After</t>
+        </is>
+      </c>
+      <c r="C57" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ? ? ? ? ????? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="D57" s="9" t="inlineStr">
+        <is>
+          <t>429 ??, ApiExceptionHandler</t>
+        </is>
+      </c>
+      <c r="E57" s="9" t="inlineStr">
+        <is>
+          <t>??? ??? ?? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="F57" s="9" t="inlineStr">
+        <is>
+          <t>429 + Retry-After: 30</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="inlineStr">
+        <is>
+          <t>?????? ???? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H57" s="9" t="inlineStr">
+        <is>
+          <t>API-008-429-BUDGET</t>
+        </is>
+      </c>
+      <c r="I57" s="9" t="inlineStr">
+        <is>
+          <t>429 ?? ?? ? ??</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K57" s="2" t="n"/>
       <c r="L57" s="2" t="n"/>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n"/>
-      <c r="B58" s="2" t="n"/>
-      <c r="C58" s="2" t="n"/>
-      <c r="D58" s="2" t="n"/>
-      <c r="E58" s="2" t="n"/>
-      <c r="F58" s="2" t="n"/>
-      <c r="G58" s="2" t="n"/>
-      <c r="H58" s="2" t="n"/>
-      <c r="I58" s="2" t="n"/>
-      <c r="J58" s="2" t="n"/>
+    <row r="58" ht="68" customHeight="1">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>X-RateLimit-Limit</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ???? ??? ?? ?? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="D58" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="E58" s="7" t="inlineStr">
+        <is>
+          <t>??/?????? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="F58" s="7" t="inlineStr">
+        <is>
+          <t>X-RateLimit-Limit: 50</t>
+        </is>
+      </c>
+      <c r="G58" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ?? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H58" s="7" t="inlineStr">
+        <is>
+          <t>rate_limited_count</t>
+        </is>
+      </c>
+      <c r="I58" s="7" t="inlineStr">
+        <is>
+          <t>429 ?? ?? 3?(Limit/Remaining/Reset) ??</t>
+        </is>
+      </c>
+      <c r="J58" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K58" s="2" t="n"/>
       <c r="L58" s="2" t="n"/>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n"/>
-      <c r="B59" s="2" t="n"/>
-      <c r="C59" s="2" t="n"/>
-      <c r="D59" s="2" t="n"/>
-      <c r="E59" s="2" t="n"/>
-      <c r="F59" s="2" t="n"/>
-      <c r="G59" s="2" t="n"/>
-      <c r="H59" s="2" t="n"/>
-      <c r="I59" s="2" t="n"/>
-      <c r="J59" s="2" t="n"/>
+    <row r="59" ht="68" customHeight="1">
+      <c r="A59" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B59" s="9" t="inlineStr">
+        <is>
+          <t>first_token_ms</t>
+        </is>
+      </c>
+      <c r="C59" s="9" t="inlineStr">
+        <is>
+          <t>?? ? ? ??? ??? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="D59" s="9" t="inlineStr">
+        <is>
+          <t>SSE ?? ???</t>
+        </is>
+      </c>
+      <c r="E59" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ?? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="F59" s="9" t="inlineStr">
+        <is>
+          <t>P95 2? ? ?? ??</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ??(P95/P99) ??? ?? ? ??</t>
+        </is>
+      </c>
+      <c r="H59" s="9" t="inlineStr">
+        <is>
+          <t>sse_first_token_ms_p95</t>
+        </is>
+      </c>
+      <c r="I59" s="9" t="inlineStr">
+        <is>
+          <t>metrics_report.md?? p50/p95 ??</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K59" s="2" t="n"/>
       <c r="L59" s="2" t="n"/>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n"/>
-      <c r="B60" s="2" t="n"/>
-      <c r="C60" s="2" t="n"/>
-      <c r="D60" s="2" t="n"/>
-      <c r="E60" s="2" t="n"/>
-      <c r="F60" s="2" t="n"/>
-      <c r="G60" s="2" t="n"/>
-      <c r="H60" s="2" t="n"/>
-      <c r="I60" s="2" t="n"/>
-      <c r="J60" s="2" t="n"/>
+    <row r="60" ht="68" customHeight="1">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>reconnect_count</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>???? ? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="D60" s="7" t="inlineStr">
+        <is>
+          <t>UI-005 ??? ??/?????</t>
+        </is>
+      </c>
+      <c r="E60" s="7" t="inlineStr">
+        <is>
+          <t>???? ???? UX ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="F60" s="7" t="inlineStr">
+        <is>
+          <t>?? ??? ???? reconnect_count ??</t>
+        </is>
+      </c>
+      <c r="G60" s="7" t="inlineStr">
+        <is>
+          <t>??? ???? ?? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H60" s="7" t="inlineStr">
+        <is>
+          <t>resume_success_rate</t>
+        </is>
+      </c>
+      <c r="I60" s="7" t="inlineStr">
+        <is>
+          <t>??? reconnect ?? ??</t>
+        </is>
+      </c>
+      <c r="J60" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K60" s="2" t="n"/>
       <c r="L60" s="2" t="n"/>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n"/>
-      <c r="B61" s="2" t="n"/>
-      <c r="C61" s="2" t="n"/>
-      <c r="D61" s="2" t="n"/>
-      <c r="E61" s="2" t="n"/>
-      <c r="F61" s="2" t="n"/>
-      <c r="G61" s="2" t="n"/>
-      <c r="H61" s="2" t="n"/>
-      <c r="I61" s="2" t="n"/>
-      <c r="J61" s="2" t="n"/>
+    <row r="61" ht="68" customHeight="1">
+      <c r="A61" s="5" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>Rate Limiter</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ? ???? ??? ???? ?? ????</t>
+        </is>
+      </c>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>API-007 ?? ???</t>
+        </is>
+      </c>
+      <c r="E61" s="5" t="inlineStr">
+        <is>
+          <t>??? ???? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="F61" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ? ?? 429 ??</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>IP? ???? ??? ?? ???/?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H61" s="5" t="inlineStr">
+        <is>
+          <t>rate_limited_count</t>
+        </is>
+      </c>
+      <c r="I61" s="5" t="inlineStr">
+        <is>
+          <t>429 ??? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J61" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K61" s="2" t="n"/>
       <c r="L61" s="2" t="n"/>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n"/>
-      <c r="B62" s="2" t="n"/>
-      <c r="C62" s="2" t="n"/>
-      <c r="D62" s="2" t="n"/>
-      <c r="E62" s="2" t="n"/>
-      <c r="F62" s="2" t="n"/>
-      <c r="G62" s="2" t="n"/>
-      <c r="H62" s="2" t="n"/>
-      <c r="I62" s="2" t="n"/>
-      <c r="J62" s="2" t="n"/>
+    <row r="62" ht="68" customHeight="1">
+      <c r="A62" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B62" s="9" t="inlineStr">
+        <is>
+          <t>Policy Engine</t>
+        </is>
+      </c>
+      <c r="C62" s="9" t="inlineStr">
+        <is>
+          <t>??? ??/?? ??? ??? ?????? ???? ??</t>
+        </is>
+      </c>
+      <c r="D62" s="9" t="inlineStr">
+        <is>
+          <t>API-008, Budget Service</t>
+        </is>
+      </c>
+      <c r="E62" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ?? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="F62" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ? safe ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H62" s="9" t="inlineStr">
+        <is>
+          <t>token_budget_exceeded_count</t>
+        </is>
+      </c>
+      <c r="I62" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ?? ???</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K62" s="2" t="n"/>
       <c r="L62" s="2" t="n"/>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n"/>
-      <c r="B63" s="2" t="n"/>
-      <c r="C63" s="2" t="n"/>
-      <c r="D63" s="2" t="n"/>
-      <c r="E63" s="2" t="n"/>
-      <c r="F63" s="2" t="n"/>
-      <c r="G63" s="2" t="n"/>
-      <c r="H63" s="2" t="n"/>
-      <c r="I63" s="2" t="n"/>
-      <c r="J63" s="2" t="n"/>
+    <row r="63" ht="68" customHeight="1">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>SpringAiToolCallingService</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ??? ????????? ???</t>
+        </is>
+      </c>
+      <c r="D63" s="7" t="inlineStr">
+        <is>
+          <t>tool/application</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ?? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="F63" s="7" t="inlineStr">
+        <is>
+          <t>policy_lookup tool ?? ??? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="G63" s="7" t="inlineStr">
+        <is>
+          <t>????? ?? ???? ?? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="H63" s="7" t="inlineStr">
+        <is>
+          <t>tool_call_ms, tool_error_rate</t>
+        </is>
+      </c>
+      <c r="I63" s="7" t="inlineStr">
+        <is>
+          <t>tool ???? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J63" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K63" s="2" t="n"/>
       <c r="L63" s="2" t="n"/>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n"/>
-      <c r="B64" s="2" t="n"/>
-      <c r="C64" s="2" t="n"/>
-      <c r="D64" s="2" t="n"/>
-      <c r="E64" s="2" t="n"/>
-      <c r="F64" s="2" t="n"/>
-      <c r="G64" s="2" t="n"/>
-      <c r="H64" s="2" t="n"/>
-      <c r="I64" s="2" t="n"/>
-      <c r="J64" s="2" t="n"/>
+    <row r="64" ht="68" customHeight="1">
+      <c r="A64" s="5" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B64" s="5" t="inlineStr">
+        <is>
+          <t>ToolContext</t>
+        </is>
+      </c>
+      <c r="C64" s="5" t="inlineStr">
+        <is>
+          <t>?? ????? ?? ??? ? ?? ??? ???? ??? ????</t>
+        </is>
+      </c>
+      <c r="D64" s="5" t="inlineStr">
+        <is>
+          <t>Spring AI tool calling</t>
+        </is>
+      </c>
+      <c r="E64" s="5" t="inlineStr">
+        <is>
+          <t>secret/tenant/role ??? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F64" s="5" t="inlineStr">
+        <is>
+          <t>tenant_key, trace_id? ToolContext?? ??</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="inlineStr">
+        <is>
+          <t>???? ??? ??? PII/??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H64" s="5" t="inlineStr">
+        <is>
+          <t>TOOL-002</t>
+        </is>
+      </c>
+      <c r="I64" s="5" t="inlineStr">
+        <is>
+          <t>tool payload? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="J64" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K64" s="2" t="n"/>
       <c r="L64" s="2" t="n"/>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n"/>
-      <c r="B65" s="2" t="n"/>
-      <c r="C65" s="2" t="n"/>
-      <c r="D65" s="2" t="n"/>
-      <c r="E65" s="2" t="n"/>
-      <c r="F65" s="2" t="n"/>
-      <c r="G65" s="2" t="n"/>
-      <c r="H65" s="2" t="n"/>
-      <c r="I65" s="2" t="n"/>
-      <c r="J65" s="2" t="n"/>
+    <row r="65" ht="68" customHeight="1">
+      <c r="A65" s="5" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>secret_ref</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
+        <is>
+          <t>??? ?? ?? Vault/KMS ?? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="D65" s="5" t="inlineStr">
+        <is>
+          <t>?? ?/?? ? ??</t>
+        </is>
+      </c>
+      <c r="E65" s="5" t="inlineStr">
+        <is>
+          <t>??? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="F65" s="5" t="inlineStr">
+        <is>
+          <t>API Key? ???? ?? secret_ref? DB? ??</t>
+        </is>
+      </c>
+      <c r="G65" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ??? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H65" s="5" t="inlineStr">
+        <is>
+          <t>SEC-003, ADM-102</t>
+        </is>
+      </c>
+      <c r="I65" s="5" t="inlineStr">
+        <is>
+          <t>DB? ?? ? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J65" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K65" s="2" t="n"/>
       <c r="L65" s="2" t="n"/>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n"/>
-      <c r="B66" s="2" t="n"/>
-      <c r="C66" s="2" t="n"/>
-      <c r="D66" s="2" t="n"/>
-      <c r="E66" s="2" t="n"/>
-      <c r="F66" s="2" t="n"/>
-      <c r="G66" s="2" t="n"/>
-      <c r="H66" s="2" t="n"/>
-      <c r="I66" s="2" t="n"/>
-      <c r="J66" s="2" t="n"/>
+    <row r="66" ht="68" customHeight="1">
+      <c r="A66" s="9" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B66" s="9" t="inlineStr">
+        <is>
+          <t>Problem Details</t>
+        </is>
+      </c>
+      <c r="C66" s="9" t="inlineStr">
+        <is>
+          <t>HTTP ??? ???? ??? ???? ???? ??</t>
+        </is>
+      </c>
+      <c r="D66" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ??</t>
+        </is>
+      </c>
+      <c r="E66" s="9" t="inlineStr">
+        <is>
+          <t>?????/???? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="F66" s="9" t="inlineStr">
+        <is>
+          <t>?? 4xx/5xx? ?? envelope? ??</t>
+        </is>
+      </c>
+      <c r="G66" s="9" t="inlineStr">
+        <is>
+          <t>?? API? ???? UX/????? ???</t>
+        </is>
+      </c>
+      <c r="H66" s="9" t="inlineStr">
+        <is>
+          <t>COM-ERROR-FORMAT</t>
+        </is>
+      </c>
+      <c r="I66" s="9" t="inlineStr">
+        <is>
+          <t>?? API 3? ?? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K66" s="2" t="n"/>
       <c r="L66" s="2" t="n"/>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n"/>
-      <c r="B67" s="2" t="n"/>
-      <c r="C67" s="2" t="n"/>
-      <c r="D67" s="2" t="n"/>
-      <c r="E67" s="2" t="n"/>
-      <c r="F67" s="2" t="n"/>
-      <c r="G67" s="2" t="n"/>
-      <c r="H67" s="2" t="n"/>
-      <c r="I67" s="2" t="n"/>
-      <c r="J67" s="2" t="n"/>
+    <row r="67" ht="68" customHeight="1">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>WebFlux</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ??? ??? ??? ???? ? ??</t>
+        </is>
+      </c>
+      <c r="D67" s="7" t="inlineStr">
+        <is>
+          <t>SSE ????? ?? ??</t>
+        </is>
+      </c>
+      <c r="E67" s="7" t="inlineStr">
+        <is>
+          <t>???? ???? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F67" s="7" t="inlineStr">
+        <is>
+          <t>?? SSE ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G67" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ? ??? ???</t>
+        </is>
+      </c>
+      <c r="H67" s="7" t="inlineStr">
+        <is>
+          <t>sse_conn_count, sse_drop_rate</t>
+        </is>
+      </c>
+      <c r="I67" s="7" t="inlineStr">
+        <is>
+          <t>?? ???? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="J67" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K67" s="2" t="n"/>
       <c r="L67" s="2" t="n"/>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n"/>
-      <c r="B68" s="2" t="n"/>
-      <c r="C68" s="2" t="n"/>
-      <c r="D68" s="2" t="n"/>
-      <c r="E68" s="2" t="n"/>
-      <c r="F68" s="2" t="n"/>
-      <c r="G68" s="2" t="n"/>
-      <c r="H68" s="2" t="n"/>
-      <c r="I68" s="2" t="n"/>
-      <c r="J68" s="2" t="n"/>
+    <row r="68" ht="68" customHeight="1">
+      <c r="A68" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B68" s="9" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="C68" s="9" t="inlineStr">
+        <is>
+          <t>?????? ???? ??? Prometheus/????? ???? ?? ?????</t>
+        </is>
+      </c>
+      <c r="D68" s="9" t="inlineStr">
+        <is>
+          <t>API/SSE/RAG ?? ???</t>
+        </is>
+      </c>
+      <c r="E68" s="9" t="inlineStr">
+        <is>
+          <t>SLO ??? ??? ???? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="F68" s="9" t="inlineStr">
+        <is>
+          <t>http_server_requests_seconds, rerank_ms ??</t>
+        </is>
+      </c>
+      <c r="G68" s="9" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ? ??? ????? ??</t>
+        </is>
+      </c>
+      <c r="H68" s="9" t="inlineStr">
+        <is>
+          <t>P95, error_rate</t>
+        </is>
+      </c>
+      <c r="I68" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ??/?? ??</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K68" s="2" t="n"/>
       <c r="L68" s="2" t="n"/>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n"/>
-      <c r="B69" s="2" t="n"/>
-      <c r="C69" s="2" t="n"/>
-      <c r="D69" s="2" t="n"/>
-      <c r="E69" s="2" t="n"/>
-      <c r="F69" s="2" t="n"/>
-      <c r="G69" s="2" t="n"/>
-      <c r="H69" s="2" t="n"/>
-      <c r="I69" s="2" t="n"/>
-      <c r="J69" s="2" t="n"/>
+    <row r="69" ht="68" customHeight="1">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>OpenSearch</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>????? ??? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="D69" s="7" t="inlineStr">
+        <is>
+          <t>?? ??/?? ??</t>
+        </is>
+      </c>
+      <c r="E69" s="7" t="inlineStr">
+        <is>
+          <t>??? ????? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F69" s="7" t="inlineStr">
+        <is>
+          <t>?? ?????? trace_id ?? ??</t>
+        </is>
+      </c>
+      <c r="G69" s="7" t="inlineStr">
+        <is>
+          <t>??? ??? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H69" s="7" t="inlineStr">
+        <is>
+          <t>log_search_ms</t>
+        </is>
+      </c>
+      <c r="I69" s="7" t="inlineStr">
+        <is>
+          <t>? ???/?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J69" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K69" s="2" t="n"/>
       <c r="L69" s="2" t="n"/>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n"/>
-      <c r="B70" s="2" t="n"/>
-      <c r="C70" s="2" t="n"/>
-      <c r="D70" s="2" t="n"/>
-      <c r="E70" s="2" t="n"/>
-      <c r="F70" s="2" t="n"/>
-      <c r="G70" s="2" t="n"/>
-      <c r="H70" s="2" t="n"/>
-      <c r="I70" s="2" t="n"/>
-      <c r="J70" s="2" t="n"/>
+    <row r="70" ht="68" customHeight="1">
+      <c r="A70" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B70" s="9" t="inlineStr">
+        <is>
+          <t>pgvector</t>
+        </is>
+      </c>
+      <c r="C70" s="9" t="inlineStr">
+        <is>
+          <t>PostgreSQL?? ?? ??? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="D70" s="9" t="inlineStr">
+        <is>
+          <t>KB ??? ??</t>
+        </is>
+      </c>
+      <c r="E70" s="9" t="inlineStr">
+        <is>
+          <t>DB ??? ???? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="F70" s="9" t="inlineStr">
+        <is>
+          <t>embedding vector(1536) ??? ??</t>
+        </is>
+      </c>
+      <c r="G70" s="9" t="inlineStr">
+        <is>
+          <t>???????? ?? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="H70" s="9" t="inlineStr">
+        <is>
+          <t>vector_ms</t>
+        </is>
+      </c>
+      <c r="I70" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ?? ??/??? ??</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K70" s="2" t="n"/>
       <c r="L70" s="2" t="n"/>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n"/>
-      <c r="B71" s="2" t="n"/>
-      <c r="C71" s="2" t="n"/>
-      <c r="D71" s="2" t="n"/>
-      <c r="E71" s="2" t="n"/>
-      <c r="F71" s="2" t="n"/>
-      <c r="G71" s="2" t="n"/>
-      <c r="H71" s="2" t="n"/>
-      <c r="I71" s="2" t="n"/>
-      <c r="J71" s="2" t="n"/>
+    <row r="71" ht="68" customHeight="1">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>ivfflat</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ??? ??? ?? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="D71" s="7" t="inlineStr">
+        <is>
+          <t>pgvector ???</t>
+        </is>
+      </c>
+      <c r="E71" s="7" t="inlineStr">
+        <is>
+          <t>???? ??? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F71" s="7" t="inlineStr">
+        <is>
+          <t>ivfflat lists=100 ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="G71" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ? ??? ??</t>
+        </is>
+      </c>
+      <c r="H71" s="7" t="inlineStr">
+        <is>
+          <t>vector_ms, recall</t>
+        </is>
+      </c>
+      <c r="I71" s="7" t="inlineStr">
+        <is>
+          <t>??? ??/????? ?? ??</t>
+        </is>
+      </c>
+      <c r="J71" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K71" s="2" t="n"/>
       <c r="L71" s="2" t="n"/>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n"/>
-      <c r="B72" s="2" t="n"/>
-      <c r="C72" s="2" t="n"/>
-      <c r="D72" s="2" t="n"/>
-      <c r="E72" s="2" t="n"/>
-      <c r="F72" s="2" t="n"/>
-      <c r="G72" s="2" t="n"/>
-      <c r="H72" s="2" t="n"/>
-      <c r="I72" s="2" t="n"/>
-      <c r="J72" s="2" t="n"/>
+    <row r="72" ht="68" customHeight="1">
+      <c r="A72" s="9" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B72" s="9" t="inlineStr">
+        <is>
+          <t>dead-letter</t>
+        </is>
+      </c>
+      <c r="C72" s="9" t="inlineStr">
+        <is>
+          <t>????? ??? ??? ?? ???? ?? ?</t>
+        </is>
+      </c>
+      <c r="D72" s="9" t="inlineStr">
+        <is>
+          <t>???/?? ?????</t>
+        </is>
+      </c>
+      <c r="E72" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ?? ???? ??? ??</t>
+        </is>
+      </c>
+      <c r="F72" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ??? dead-letter? ??</t>
+        </is>
+      </c>
+      <c r="G72" s="9" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ????? ??? ?? ???</t>
+        </is>
+      </c>
+      <c r="H72" s="9" t="inlineStr">
+        <is>
+          <t>index_success_rate, reindex_count</t>
+        </is>
+      </c>
+      <c r="I72" s="9" t="inlineStr">
+        <is>
+          <t>dead-letter ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K72" s="2" t="n"/>
       <c r="L72" s="2" t="n"/>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n"/>
-      <c r="B73" s="2" t="n"/>
-      <c r="C73" s="2" t="n"/>
-      <c r="D73" s="2" t="n"/>
-      <c r="E73" s="2" t="n"/>
-      <c r="F73" s="2" t="n"/>
-      <c r="G73" s="2" t="n"/>
-      <c r="H73" s="2" t="n"/>
-      <c r="I73" s="2" t="n"/>
-      <c r="J73" s="2" t="n"/>
+    <row r="73" ht="68" customHeight="1">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>BRIN</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>??? ??? ???? ??? ?? ???</t>
+        </is>
+      </c>
+      <c r="D73" s="7" t="inlineStr">
+        <is>
+          <t>??/??? ??? ???</t>
+        </is>
+      </c>
+      <c r="E73" s="7" t="inlineStr">
+        <is>
+          <t>????? ???? ????? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F73" s="7" t="inlineStr">
+        <is>
+          <t>created_at ?? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G73" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ?????? ???</t>
+        </is>
+      </c>
+      <c r="H73" s="7" t="inlineStr">
+        <is>
+          <t>log_search_ms</t>
+        </is>
+      </c>
+      <c r="I73" s="7" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J73" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K73" s="2" t="n"/>
       <c r="L73" s="2" t="n"/>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n"/>
-      <c r="B74" s="2" t="n"/>
-      <c r="C74" s="2" t="n"/>
-      <c r="D74" s="2" t="n"/>
-      <c r="E74" s="2" t="n"/>
-      <c r="F74" s="2" t="n"/>
-      <c r="G74" s="2" t="n"/>
-      <c r="H74" s="2" t="n"/>
-      <c r="I74" s="2" t="n"/>
-      <c r="J74" s="2" t="n"/>
+    <row r="74" ht="68" customHeight="1">
+      <c r="A74" s="5" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B74" s="5" t="inlineStr">
+        <is>
+          <t>TraceGuard</t>
+        </is>
+      </c>
+      <c r="C74" s="5" t="inlineStr">
+        <is>
+          <t>trace_id ??? ?? ??? ?? ??? ???? ??</t>
+        </is>
+      </c>
+      <c r="D74" s="5" t="inlineStr">
+        <is>
+          <t>global/observability</t>
+        </is>
+      </c>
+      <c r="E74" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ? ???? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F74" s="5" t="inlineStr">
+        <is>
+          <t>trace_id ?? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="inlineStr">
+        <is>
+          <t>?? ???? ???? ?? ???</t>
+        </is>
+      </c>
+      <c r="H74" s="5" t="inlineStr">
+        <is>
+          <t>SYS-004-409-TRACE</t>
+        </is>
+      </c>
+      <c r="I74" s="5" t="inlineStr">
+        <is>
+          <t>safe_response/error/done ??? trace ??</t>
+        </is>
+      </c>
+      <c r="J74" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K74" s="2" t="n"/>
       <c r="L74" s="2" t="n"/>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n"/>
-      <c r="B75" s="2" t="n"/>
-      <c r="C75" s="2" t="n"/>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
-      <c r="F75" s="2" t="n"/>
-      <c r="G75" s="2" t="n"/>
-      <c r="H75" s="2" t="n"/>
-      <c r="I75" s="2" t="n"/>
-      <c r="J75" s="2" t="n"/>
+    <row r="75" ht="68" customHeight="1">
+      <c r="A75" s="9" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="B75" s="9" t="inlineStr">
+        <is>
+          <t>TraceContext</t>
+        </is>
+      </c>
+      <c r="C75" s="9" t="inlineStr">
+        <is>
+          <t>?? ??? trace_id? ????? ???? ?? ????</t>
+        </is>
+      </c>
+      <c r="D75" s="9" t="inlineStr">
+        <is>
+          <t>???/??? ??</t>
+        </is>
+      </c>
+      <c r="E75" s="9" t="inlineStr">
+        <is>
+          <t>API-DB-SSE ? ?? ??? ??</t>
+        </is>
+      </c>
+      <c r="F75" s="9" t="inlineStr">
+        <is>
+          <t>DB ?? ???? ?? trace_id ??</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="inlineStr">
+        <is>
+          <t>??? ???? ???? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H75" s="9" t="inlineStr">
+        <is>
+          <t>trace_coverage_pct</t>
+        </is>
+      </c>
+      <c r="I75" s="9" t="inlineStr">
+        <is>
+          <t>?? 1?? DB/SSE trace ?? ??</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K75" s="2" t="n"/>
       <c r="L75" s="2" t="n"/>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n"/>
-      <c r="B76" s="2" t="n"/>
-      <c r="C76" s="2" t="n"/>
-      <c r="D76" s="2" t="n"/>
-      <c r="E76" s="2" t="n"/>
-      <c r="F76" s="2" t="n"/>
-      <c r="G76" s="2" t="n"/>
-      <c r="H76" s="2" t="n"/>
-      <c r="I76" s="2" t="n"/>
-      <c r="J76" s="2" t="n"/>
+    <row r="76" ht="68" customHeight="1">
+      <c r="A76" s="5" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B76" s="5" t="inlineStr">
+        <is>
+          <t>kill-switch</t>
+        </is>
+      </c>
+      <c r="C76" s="5" t="inlineStr">
+        <is>
+          <t>?? provider/??? ?? ???? ?? ???</t>
+        </is>
+      </c>
+      <c r="D76" s="5" t="inlineStr">
+        <is>
+          <t>OPS playbook, ???? API</t>
+        </is>
+      </c>
+      <c r="E76" s="5" t="inlineStr">
+        <is>
+          <t>?? ??? ?? ??? ??? ??</t>
+        </is>
+      </c>
+      <c r="F76" s="5" t="inlineStr">
+        <is>
+          <t>?? LLM provider ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="inlineStr">
+        <is>
+          <t>??/??? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H76" s="5" t="inlineStr">
+        <is>
+          <t>OPS-PROVIDER-KILLSWITCH</t>
+        </is>
+      </c>
+      <c r="I76" s="5" t="inlineStr">
+        <is>
+          <t>?? trace_id? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J76" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K76" s="2" t="n"/>
       <c r="L76" s="2" t="n"/>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n"/>
-      <c r="B77" s="2" t="n"/>
-      <c r="C77" s="2" t="n"/>
-      <c r="D77" s="2" t="n"/>
-      <c r="E77" s="2" t="n"/>
-      <c r="F77" s="2" t="n"/>
-      <c r="G77" s="2" t="n"/>
-      <c r="H77" s="2" t="n"/>
-      <c r="I77" s="2" t="n"/>
-      <c r="J77" s="2" t="n"/>
+    <row r="77" ht="68" customHeight="1">
+      <c r="A77" s="5" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B77" s="5" t="inlineStr">
+        <is>
+          <t>rollback</t>
+        </is>
+      </c>
+      <c r="C77" s="5" t="inlineStr">
+        <is>
+          <t>??? ?? ??? ?? ?? ???? ???? ?? ??</t>
+        </is>
+      </c>
+      <c r="D77" s="5" t="inlineStr">
+        <is>
+          <t>??/???/??/KB ??</t>
+        </is>
+      </c>
+      <c r="E77" s="5" t="inlineStr">
+        <is>
+          <t>??? ??? ???? ??? ???</t>
+        </is>
+      </c>
+      <c r="F77" s="5" t="inlineStr">
+        <is>
+          <t>??? ?? ?? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="G77" s="5" t="inlineStr">
+        <is>
+          <t>??? ?????? ?? ? ??? ?? ?? ??</t>
+        </is>
+      </c>
+      <c r="H77" s="5" t="inlineStr">
+        <is>
+          <t>rollback_count</t>
+        </is>
+      </c>
+      <c r="I77" s="5" t="inlineStr">
+        <is>
+          <t>?? ?? ? ?? ???? ???</t>
+        </is>
+      </c>
+      <c r="J77" s="6" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
       <c r="K77" s="2" t="n"/>
       <c r="L77" s="2" t="n"/>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n"/>
-      <c r="B78" s="2" t="n"/>
-      <c r="C78" s="2" t="n"/>
-      <c r="D78" s="2" t="n"/>
-      <c r="E78" s="2" t="n"/>
-      <c r="F78" s="2" t="n"/>
-      <c r="G78" s="2" t="n"/>
-      <c r="H78" s="2" t="n"/>
-      <c r="I78" s="2" t="n"/>
-      <c r="J78" s="2" t="n"/>
+    <row r="78" ht="68" customHeight="1">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>canary_ratio</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>? ??? ?? ????? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="D78" s="7" t="inlineStr">
+        <is>
+          <t>????/?? ??</t>
+        </is>
+      </c>
+      <c r="E78" s="7" t="inlineStr">
+        <is>
+          <t>?? ?? ?? ???? ?? ???? ??</t>
+        </is>
+      </c>
+      <c r="F78" s="7" t="inlineStr">
+        <is>
+          <t>5% -&gt; 20% -&gt; 100% ?? ??</t>
+        </is>
+      </c>
+      <c r="G78" s="7" t="inlineStr">
+        <is>
+          <t>???? ?? ???? ??? ??</t>
+        </is>
+      </c>
+      <c r="H78" s="7" t="inlineStr">
+        <is>
+          <t>canary_pass_rate, rollback_count</t>
+        </is>
+      </c>
+      <c r="I78" s="7" t="inlineStr">
+        <is>
+          <t>??? ??/?? ?? ??</t>
+        </is>
+      </c>
+      <c r="J78" s="8" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K78" s="2" t="n"/>
       <c r="L78" s="2" t="n"/>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n"/>
-      <c r="B79" s="2" t="n"/>
-      <c r="C79" s="2" t="n"/>
-      <c r="D79" s="2" t="n"/>
-      <c r="E79" s="2" t="n"/>
-      <c r="F79" s="2" t="n"/>
-      <c r="G79" s="2" t="n"/>
-      <c r="H79" s="2" t="n"/>
-      <c r="I79" s="2" t="n"/>
-      <c r="J79" s="2" t="n"/>
+    <row r="79" ht="68" customHeight="1">
+      <c r="A79" s="9" t="inlineStr">
+        <is>
+          <t>?????</t>
+        </is>
+      </c>
+      <c r="B79" s="9" t="inlineStr">
+        <is>
+          <t>provider regression</t>
+        </is>
+      </c>
+      <c r="C79" s="9" t="inlineStr">
+        <is>
+          <t>LLM ??? ??/?? ? ?? ??? ????? ???? ????</t>
+        </is>
+      </c>
+      <c r="D79" s="9" t="inlineStr">
+        <is>
+          <t>CI nightly, provider ?? ??</t>
+        </is>
+      </c>
+      <c r="E79" s="9" t="inlineStr">
+        <is>
+          <t>??/??? ???? ?? ????? ??? ?? ??</t>
+        </is>
+      </c>
+      <c r="F79" s="9" t="inlineStr">
+        <is>
+          <t>latest local SKIPPED?? latest PASS ??? SSOT? ??</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="inlineStr">
+        <is>
+          <t>SKIPPED? PASS? ???? ?? ??? ???</t>
+        </is>
+      </c>
+      <c r="H79" s="9" t="inlineStr">
+        <is>
+          <t>LLM-PROVIDER-001, PROVIDER-EVIDENCE-001</t>
+        </is>
+      </c>
+      <c r="I79" s="9" t="inlineStr">
+        <is>
+          <t>nightly ??? PASS artifact ?? ??</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K79" s="2" t="n"/>
       <c r="L79" s="2" t="n"/>
     </row>
@@ -8869,7 +10709,7 @@
       <c r="L500" s="2" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J24"/>
+  <autoFilter ref="A4:J79"/>
   <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>

</xml_diff>